<commit_message>
exportar padel usa v 1
</commit_message>
<xml_diff>
--- a/Bot/padel_usa.xlsx
+++ b/Bot/padel_usa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="142">
   <si>
     <t>Nombre</t>
   </si>
@@ -146,77 +146,598 @@
   </si>
   <si>
     <t xml:space="preserve">
- $339,99
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $279,99
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $329,99
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $389,99
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $419,99
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $429,99
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $189,95
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $229,95
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $269,95
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $109,95
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $229,00
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $144,00
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $192,00
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $250,74
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
- $307,74
+Bullpadel Hack 03 Comfort 2024
+                      Bullpadel Hack 03 Comfort 2024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bullpadel Hack 03 Hybrid 2024
+                      Bullpadel Hack 03 Hybrid 2024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Nox AT Genius LIMITED Edition Pack
+                      Nox AT Genius LIMITED Edition Pack
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Nox ML10 PRO CUP Luxury 2024 Miguel Lamperti's racket
+                      Nox ML10 PRO CUP Luxury 2024 Miguel Lamperti's racket
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Nox AT10 Luxury GENIUS 12K 2024 by Agustín Tapia
+                      Nox AT10 Luxury GENIUS 12K 2024 by Agustín Tapia
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Nox AT Genius Attack 18K 2024 by Agustín Tapia
+                      Nox AT Genius Attack 18K 2024 by Agustín Tapia
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Nox AT10 Luxury GENIUS 18K Alum 2024 by Agustín Tapia
+                      Nox AT10 Luxury GENIUS 18K Alum 2024 by Agustín Tapia
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Slazenger Panther Epic Gold
+                      Slazenger Panther Epic Gold
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Slazenger Panther Icon Hybrid Gold
+                      Slazenger Panther Icon Hybrid Gold
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Slazenger Panther Icon Pro
+                      Slazenger Panther Icon Pro
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Extreme Elite
+                      Head Extreme Elite
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Extreme Motion
+                      Head Extreme Motion
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Extreme One
+                      Head Extreme One
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Babolat Technical Vertuo
+                      Babolat Technical Vertuo
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Wilson Bela LT V2 White
+                      Wilson Bela LT V2 White
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Babolat Technical Veron
+                      Babolat Technical Veron
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Zephyr
+                      Head Zephyr
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Nox AT Genius LIMITED EDITION
+                      Nox AT Genius LIMITED EDITION
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Osaka Vision Pro Control Snap
+                      Osaka Vision Pro Control Snap
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Osaka Pro Tour Power - Limited Edition
+                      Osaka Pro Tour Power - Limited Edition
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Wilson Bela Pro v2
+                      Wilson Bela Pro v2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Babolat Counter Viper
+                      Babolat Counter Viper
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Concord 2023
+                      Head Concord 2023
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Alpha Touch Graphene 360+
+                      Head Alpha Touch Graphene 360+
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Wilson Blade Pro v2
+                      Wilson Blade Pro v2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Speed Pro
+                      Head Speed Pro
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Speed Elite
+                      Head Speed Elite
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Speed Pro X
+                      Head Speed Pro X
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Wilson Blade Elite v2
+                      Wilson Blade Elite v2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Wilson Blade Team V2
+                      Wilson Blade Team V2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Wilson Blade LT V2
+                      Wilson Blade LT V2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Babolat Air Veron
+                      Babolat Air Veron
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bullpadel IONIC CONTROL 24
+                      Bullpadel IONIC CONTROL 24
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bullpadel IONIC POWER 24
+                      Bullpadel IONIC POWER 24
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Flash Padel Racket
+                      Head Flash Padel Racket
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Zephyr UL Padel Racket
+                      Head Zephyr UL Padel Racket
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Wilson Bela Team V2
+                      Wilson Bela Team V2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bullpadel Elite W 2024
+                      Bullpadel Elite W 2024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bullpadel Flow W 2024
+                      Bullpadel Flow W 2024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bullpadel Vertex 04 Hybrid 2024
+                      Bullpadel Vertex 04 Hybrid 2024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bullpadel Vertex 04 24
+                      Bullpadel Vertex 04 24
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bullpadel Hack 03 2024
+                      Bullpadel Hack 03 2024
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Extreme Pro
+                      Head Extreme Pro
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Tecnifibre Wall Master 365
+                      Tecnifibre Wall Master 365
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Tecnifibre Wall Master 370
+                      Tecnifibre Wall Master 370
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Babolat Air Vertuo
+                      Babolat Air Vertuo
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Siux Electra ST2 Stupa Pro
+                      Siux Electra ST2 Stupa Pro
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Siux Diablo Revolution II Sanyo Pro
+                      Siux Diablo Revolution II Sanyo Pro
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Nox ML10 Pro Cup Rough Surface Edition
+                      Nox ML10 Pro Cup Rough Surface Edition
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Varlion LW PRISMA Airflow S
+                      Varlion LW PRISMA Airflow S
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Osaka Vision Pro Power Touch
+                      Osaka Vision Pro Power Touch
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Osaka Pro Tour Control Touch
+                      Osaka Pro Tour Control Touch
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Osaka Pro Tour Power Snap
+                      Osaka Pro Tour Power Snap
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Osaka Pro Tour Control - Limited Edition
+                      Osaka Pro Tour Control - Limited Edition
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Adidas Metalbone 3.2
+                      Adidas Metalbone 3.2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Head Speed Motion
+                      Head Speed Motion
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 339,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 279,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 329,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 389,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 419,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 429,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 189,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 229,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 269,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 109,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 229,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 144,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 192,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 250,74
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 307,74
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 250,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 325,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 430,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 359,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 369,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 420,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 450,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 209,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 299,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 269,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 240,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 139,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 220,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 295,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 339,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 256,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 120,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 150,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 289,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 290,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 199,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 129,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 249,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 195,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 59,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 110,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 179,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 305,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 280,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 315,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 341,94
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 330,54
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 289,95
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 190,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 249,99
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 270,00
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 199,95
 </t>
   </si>
   <si>
@@ -236,6 +757,21 @@
   </si>
   <si>
     <t>Bullpadel</t>
+  </si>
+  <si>
+    <t>Nox</t>
+  </si>
+  <si>
+    <t>Slazenger</t>
+  </si>
+  <si>
+    <t>Osaka</t>
+  </si>
+  <si>
+    <t>Tecnifibre</t>
+  </si>
+  <si>
+    <t>Varlion</t>
   </si>
 </sst>
 </file>
@@ -593,7 +1129,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -618,276 +1154,1060 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
       <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
         <v>37</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
         <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>108</v>
+      </c>
+      <c r="D42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>115</v>
+      </c>
+      <c r="D51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" t="s">
+        <v>120</v>
+      </c>
+      <c r="D58" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" t="s">
+        <v>121</v>
+      </c>
+      <c r="D59" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+      <c r="D60" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" t="s">
+        <v>126</v>
+      </c>
+      <c r="D64" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C65" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" t="s">
+        <v>89</v>
+      </c>
+      <c r="D68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+      <c r="C69" t="s">
+        <v>128</v>
+      </c>
+      <c r="D69" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70" t="s">
+        <v>111</v>
+      </c>
+      <c r="D70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72" t="s">
+        <v>127</v>
+      </c>
+      <c r="D72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" t="s">
+        <v>129</v>
+      </c>
+      <c r="D73" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74" t="s">
+        <v>94</v>
+      </c>
+      <c r="D74" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75" t="s">
+        <v>107</v>
+      </c>
+      <c r="D75" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" t="s">
+        <v>94</v>
+      </c>
+      <c r="D76" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77" t="s">
+        <v>130</v>
+      </c>
+      <c r="D77" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>